<commit_message>
Add massage therapist to schema
</commit_message>
<xml_diff>
--- a/docs/Appointment Table.xlsx
+++ b/docs/Appointment Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\schedular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\schedular\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07226B84-77EA-4F49-821E-DBBE130B0256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2872C036-DD03-48F4-A962-C414F1BF6B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="3750" windowWidth="27990" windowHeight="16710" activeTab="3" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
+    <workbookView xWindow="990" yWindow="4035" windowWidth="26910" windowHeight="16170" activeTab="3" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
   <si>
     <t>Attributes</t>
   </si>
@@ -517,6 +517,15 @@
   </si>
   <si>
     <t>PK = pk</t>
+  </si>
+  <si>
+    <t>administratorId</t>
+  </si>
+  <si>
+    <t>administratorDetails</t>
+  </si>
+  <si>
+    <t>{ …admin }</t>
   </si>
 </sst>
 </file>
@@ -748,10 +757,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1484,7 +1493,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="F17" sqref="F17:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,18 +1513,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -1530,12 +1539,12 @@
       <c r="B2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -1543,10 +1552,10 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="40" t="s">
         <v>86</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -1559,15 +1568,21 @@
         <v>66</v>
       </c>
       <c r="F3" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="K3" s="32" t="s">
         <v>118</v>
       </c>
       <c r="L3" s="17"/>
@@ -1575,8 +1590,8 @@
       <c r="N3" s="19"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
@@ -1586,24 +1601,30 @@
       <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="7">
         <v>60</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I4" s="33"/>
+      <c r="K4" s="33"/>
       <c r="L4" s="21"/>
       <c r="N4" s="22"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="40" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="16" t="s">
@@ -1621,18 +1642,17 @@
       <c r="G5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="J5" s="21"/>
+      <c r="K5" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="20"/>
       <c r="L5" s="22"/>
       <c r="M5" s="21"/>
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1648,18 +1668,17 @@
       <c r="G6" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="33"/>
       <c r="J6" s="21"/>
-      <c r="K6" s="20"/>
+      <c r="K6" s="33"/>
       <c r="L6" s="22"/>
       <c r="M6" s="21"/>
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="40" t="s">
         <v>88</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -1672,19 +1691,25 @@
         <v>66</v>
       </c>
       <c r="F7" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="20"/>
+      <c r="K7" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="K7" s="21"/>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
       <c r="O7" s="23"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1694,20 +1719,26 @@
       <c r="E8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="7">
         <v>60</v>
       </c>
-      <c r="I8" s="37"/>
-      <c r="K8" s="21"/>
+      <c r="I8" s="20"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
       <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="40" t="s">
         <v>89</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -1720,19 +1751,25 @@
         <v>66</v>
       </c>
       <c r="F9" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="20"/>
+      <c r="K9" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="K9" s="21"/>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
       <c r="O9" s="22"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1742,20 +1779,26 @@
       <c r="E10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="7">
         <v>60</v>
       </c>
-      <c r="I10" s="37"/>
-      <c r="K10" s="21"/>
+      <c r="I10" s="20"/>
+      <c r="K10" s="37"/>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
       <c r="O10" s="22"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="40" t="s">
         <v>87</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -1767,26 +1810,21 @@
       <c r="E11" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="16" t="s">
+      <c r="I11" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="J11" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="K11" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
       <c r="L11" s="21"/>
       <c r="N11" s="22"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1796,26 +1834,21 @@
       <c r="E12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="7">
-        <v>60</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="I12" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I12" s="33"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
+      <c r="K12" s="33"/>
       <c r="L12" s="21"/>
       <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="40" t="s">
         <v>87</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -1833,19 +1866,18 @@
       <c r="G13" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="34" t="s">
+      <c r="J13" s="21"/>
+      <c r="K13" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="20"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
       <c r="P13" s="24"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="5" t="s">
         <v>106</v>
       </c>
@@ -1861,19 +1893,18 @@
       <c r="G14" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="35"/>
       <c r="J14" s="21"/>
-      <c r="K14" s="20"/>
+      <c r="K14" s="35"/>
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
       <c r="P14" s="24"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="40" t="s">
         <v>87</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1891,19 +1922,18 @@
       <c r="G15" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I15" s="32" t="s">
+      <c r="J15" s="21"/>
+      <c r="K15" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="20"/>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
       <c r="P15" s="24"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="5" t="s">
         <v>12</v>
       </c>
@@ -1919,19 +1949,18 @@
       <c r="G16" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I16" s="33"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="20"/>
+      <c r="K16" s="33"/>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
       <c r="P16" s="24"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="40" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="16" t="s">
@@ -1944,19 +1973,24 @@
         <v>66</v>
       </c>
       <c r="F17" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="36" t="s">
+      <c r="K17" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="K17" s="21"/>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="O17" s="22"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
@@ -1966,20 +2000,25 @@
       <c r="E18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" s="7">
         <v>60</v>
       </c>
-      <c r="I18" s="37"/>
-      <c r="K18" s="21"/>
+      <c r="K18" s="37"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="O18" s="22"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="40" t="s">
         <v>107</v>
       </c>
       <c r="C19" s="16" t="s">
@@ -1994,17 +2033,16 @@
       <c r="F19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="38" t="s">
+      <c r="K19" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="K19" s="21"/>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
       <c r="O19" s="22"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="7" t="s">
         <v>108</v>
       </c>
@@ -2017,15 +2055,14 @@
       <c r="F20" s="7">
         <v>7805555555</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="K20" s="20"/>
+      <c r="K20" s="38"/>
       <c r="O20" s="22"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="40" t="s">
         <v>111</v>
       </c>
       <c r="C21" s="16" t="s">
@@ -2040,17 +2077,16 @@
       <c r="F21" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I21" s="38" t="s">
+      <c r="K21" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="K21" s="21"/>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
       <c r="O21" s="22"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="7" t="s">
         <v>112</v>
       </c>
@@ -2063,8 +2099,7 @@
       <c r="F22" s="7">
         <v>7808888888</v>
       </c>
-      <c r="I22" s="39"/>
-      <c r="K22" s="20"/>
+      <c r="K22" s="39"/>
       <c r="O22" s="22"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2308,6 +2343,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="A21:A22"/>
@@ -2324,12 +2365,6 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E20" r:id="rId1" xr:uid="{B610ACA8-BB27-4EB4-9FA5-FD775FD9DEC9}"/>

</xml_diff>

<commit_message>
Add Booking Reminder notifications (#23)
* Rename getBookings to getUserBookings

* Add getBookings

* Add context

* Split out stacks

* Context

* Clean up

* Add lambda to query dynamodb for upcoming appointments

* Update to tomorrows date

* Send events

* WIP EventBridge

* Hook up EventBridge

* Rename and update to send email
gp

* Email

* Email

* Send email

* Enable appts
</commit_message>
<xml_diff>
--- a/docs/Appointment Table.xlsx
+++ b/docs/Appointment Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\schedular\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AMAABCA\eric-bach\schedular\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2872C036-DD03-48F4-A962-C414F1BF6B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA233EC6-5EDC-4CEF-A48A-D09D03E5151D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="4035" windowWidth="26910" windowHeight="16170" activeTab="3" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
+    <workbookView xWindow="6630" yWindow="2910" windowWidth="35190" windowHeight="20250" activeTab="3" xr2:uid="{6AC31791-E6D3-4762-A3D2-8A55CA9F95FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="142">
   <si>
     <t>Attributes</t>
   </si>
@@ -414,9 +414,6 @@
     <t>Create booking</t>
   </si>
   <si>
-    <t>createAppointment</t>
-  </si>
-  <si>
     <t>getAvailableAppointments</t>
   </si>
   <si>
@@ -516,9 +513,6 @@
     <t>pk</t>
   </si>
   <si>
-    <t>PK = pk</t>
-  </si>
-  <si>
     <t>administratorId</t>
   </si>
   <si>
@@ -526,6 +520,45 @@
   </si>
   <si>
     <t>{ …admin }</t>
+  </si>
+  <si>
+    <t>getUserBookings</t>
+  </si>
+  <si>
+    <t>Get booked bookings by date</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>type = booking, SK startsWith &lt;date&gt;</t>
+  </si>
+  <si>
+    <t>appointmentDetails.status = booked</t>
+  </si>
+  <si>
+    <t>createAppointments</t>
+  </si>
+  <si>
+    <t>Create appointments</t>
+  </si>
+  <si>
+    <t>deleteAppointments</t>
+  </si>
+  <si>
+    <t>Delete appointments</t>
+  </si>
+  <si>
+    <t>getAppointment</t>
+  </si>
+  <si>
+    <t>Get appointment by id</t>
+  </si>
+  <si>
+    <t>PK = appt#&lt;apptId&gt;</t>
+  </si>
+  <si>
+    <t>PK = booking#&lt;bookingId&gt;</t>
   </si>
 </sst>
 </file>
@@ -640,7 +673,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -757,11 +790,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1490,10 +1526,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E548137-E7BE-486B-96A5-865A1089DC79}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:H18"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,7 +1540,7 @@
     <col min="4" max="4" width="11.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34" style="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" style="20" bestFit="1" customWidth="1"/>
@@ -1513,18 +1549,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -1539,12 +1575,12 @@
       <c r="B2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -1552,10 +1588,10 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>86</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -1568,30 +1604,30 @@
         <v>66</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J3" s="16" t="s">
         <v>53</v>
       </c>
       <c r="K3" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L3" s="17"/>
       <c r="M3" s="18"/>
       <c r="N3" s="19"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
@@ -1605,7 +1641,7 @@
         <v>57</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H4" s="7">
         <v>60</v>
@@ -1614,17 +1650,17 @@
         <v>56</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K4" s="33"/>
       <c r="L4" s="21"/>
       <c r="N4" s="22"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="41" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="16" t="s">
@@ -1644,15 +1680,15 @@
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L5" s="22"/>
       <c r="M5" s="21"/>
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1663,10 +1699,10 @@
         <v>57</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="33"/>
@@ -1675,10 +1711,10 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="41" t="s">
         <v>88</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -1691,25 +1727,25 @@
         <v>66</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="20"/>
       <c r="K7" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
       <c r="O7" s="23"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1723,7 +1759,7 @@
         <v>57</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H8" s="7">
         <v>60</v>
@@ -1735,10 +1771,10 @@
       <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="41" t="s">
         <v>89</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -1751,25 +1787,25 @@
         <v>66</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="20"/>
       <c r="K9" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
       <c r="O9" s="22"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1783,7 +1819,7 @@
         <v>57</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H10" s="7">
         <v>60</v>
@@ -1795,10 +1831,10 @@
       <c r="O10" s="22"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -1811,20 +1847,20 @@
         <v>66</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J11" s="16" t="s">
         <v>53</v>
       </c>
       <c r="K11" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L11" s="21"/>
       <c r="N11" s="22"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1838,17 +1874,17 @@
         <v>56</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K12" s="33"/>
       <c r="L12" s="21"/>
       <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -1868,7 +1904,7 @@
       </c>
       <c r="J13" s="21"/>
       <c r="K13" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
@@ -1876,10 +1912,10 @@
       <c r="P13" s="24"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>78</v>
@@ -1888,10 +1924,10 @@
         <v>57</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J14" s="21"/>
       <c r="K14" s="35"/>
@@ -1901,10 +1937,10 @@
       <c r="P14" s="24"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1924,7 +1960,7 @@
       </c>
       <c r="J15" s="21"/>
       <c r="K15" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
@@ -1932,8 +1968,8 @@
       <c r="P15" s="24"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="5" t="s">
         <v>12</v>
       </c>
@@ -1944,10 +1980,10 @@
         <v>57</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J16" s="21"/>
       <c r="K16" s="33"/>
@@ -1957,10 +1993,10 @@
       <c r="P16" s="24"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="16" t="s">
@@ -1973,24 +2009,24 @@
         <v>66</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H17" s="16" t="s">
         <v>10</v>
       </c>
       <c r="K17" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="O17" s="22"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
@@ -2004,7 +2040,7 @@
         <v>57</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H18" s="7">
         <v>60</v>
@@ -2015,11 +2051,11 @@
       <c r="O18" s="22"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="40" t="s">
-        <v>107</v>
+      <c r="B19" s="41" t="s">
+        <v>106</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>58</v>
@@ -2034,23 +2070,23 @@
         <v>60</v>
       </c>
       <c r="K19" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
       <c r="O19" s="22"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="E20" s="25" t="s">
         <v>109</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>110</v>
       </c>
       <c r="F20" s="7">
         <v>7805555555</v>
@@ -2059,11 +2095,11 @@
       <c r="O20" s="22"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="40" t="s">
-        <v>111</v>
+      <c r="B21" s="41" t="s">
+        <v>110</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>58</v>
@@ -2078,23 +2114,23 @@
         <v>60</v>
       </c>
       <c r="K21" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
       <c r="O21" s="22"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="25" t="s">
         <v>112</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>113</v>
       </c>
       <c r="F22" s="7">
         <v>7808888888</v>
@@ -2142,10 +2178,10 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>49</v>
+        <v>135</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>48</v>
@@ -2165,190 +2201,261 @@
       </c>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>95</v>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>136</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>24</v>
+        <v>137</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>114</v>
+        <v>48</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" s="28" t="s">
-        <v>104</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="H27" s="28"/>
       <c r="I27" s="28" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K27" s="21"/>
     </row>
-    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>96</v>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="42" t="s">
+        <v>138</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="21"/>
+    </row>
+    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E29" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="H28" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="I28" s="28" t="s">
+      <c r="H29" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="I29" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="J28" s="20" t="s">
+      <c r="J29" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K28" s="21"/>
-    </row>
-    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="K29" s="29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
-        <v>124</v>
+      <c r="K29" s="21"/>
+    </row>
+    <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="42" t="s">
+        <v>94</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>125</v>
+        <v>24</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>113</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>127</v>
+        <v>114</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>13</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>19</v>
       </c>
+      <c r="K30" s="21"/>
     </row>
     <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
-        <v>98</v>
+      <c r="A31" s="42" t="s">
+        <v>96</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>102</v>
+        <v>48</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="H31" s="28" t="s">
-        <v>104</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="H31" s="28"/>
       <c r="I31" s="28" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J31" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="K31" s="21"/>
-    </row>
-    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
-        <v>99</v>
+      <c r="K31" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="42" t="s">
+        <v>123</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>48</v>
+        <v>6</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>125</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28" t="s">
-        <v>63</v>
+      <c r="F32" s="20" t="s">
+        <v>141</v>
       </c>
       <c r="J32" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="K32" s="29" t="s">
+    </row>
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="I34" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34" s="21"/>
+    </row>
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="J35" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" s="29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="31"/>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="A21:A22"/>
@@ -2365,6 +2472,12 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E20" r:id="rId1" xr:uid="{B610ACA8-BB27-4EB4-9FA5-FD775FD9DEC9}"/>

</xml_diff>